<commit_message>
Remove lock file, rename average and overall accuracy
</commit_message>
<xml_diff>
--- a/result/outcome_statistics_inception.xlsx
+++ b/result/outcome_statistics_inception.xlsx
@@ -16,12 +16,12 @@
     <sheet name="outcome_stats_inception_avg" sheetId="2" r:id="rId2"/>
     <sheet name="outcome_stats_inception_final" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="158">
   <si>
     <t>building_class</t>
   </si>
@@ -479,9 +479,6 @@
     <t>FOV</t>
   </si>
   <si>
-    <t>TA</t>
-  </si>
-  <si>
     <t>OA</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>avg (sd.)</t>
+  </si>
+  <si>
+    <t>AA</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1513,7 +1523,7 @@
         <v>0.96936041108278659</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="R2:W2" si="0">AVERAGE(J2:J5)</f>
+        <f t="shared" ref="S2:W2" si="0">AVERAGE(J2:J5)</f>
         <v>0.84489453247979762</v>
       </c>
       <c r="T2">
@@ -1778,7 +1788,7 @@
         <v>0.44793088756101074</v>
       </c>
       <c r="R6">
-        <f t="shared" ref="Q6:R6" si="3">AVERAGE(I6:I9)</f>
+        <f t="shared" ref="R6" si="3">AVERAGE(I6:I9)</f>
         <v>0.97277686036639976</v>
       </c>
       <c r="S6">
@@ -1802,31 +1812,31 @@
         <v>0.91660440457402204</v>
       </c>
       <c r="Y6" t="str">
-        <f t="shared" ref="Y6:Y37" si="9">TEXT(Q6, "0.00") &amp; "  (" &amp; TEXT( Q7, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y6" si="9">TEXT(Q6, "0.00") &amp; "  (" &amp; TEXT( Q7, "0.00") &amp; ")"</f>
         <v>0.45  (0.02)</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" ref="Z6:Z69" si="10">TEXT(R6, "0.00") &amp; "  (" &amp; TEXT( R7, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z6" si="10">TEXT(R6, "0.00") &amp; "  (" &amp; TEXT( R7, "0.00") &amp; ")"</f>
         <v>0.97  (0.00)</v>
       </c>
       <c r="AA6" t="str">
-        <f t="shared" ref="AA6:AA69" si="11">TEXT(S6, "0.00") &amp; "  (" &amp; TEXT( S7, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA6" si="11">TEXT(S6, "0.00") &amp; "  (" &amp; TEXT( S7, "0.00") &amp; ")"</f>
         <v>0.87  (0.02)</v>
       </c>
       <c r="AB6" t="str">
-        <f t="shared" ref="AB6:AB37" si="12">TEXT(T6, "0") &amp; "  (" &amp; TEXT( T7, "0") &amp; ")"</f>
+        <f t="shared" ref="AB6" si="12">TEXT(T6, "0") &amp; "  (" &amp; TEXT( T7, "0") &amp; ")"</f>
         <v>2120  (446)</v>
       </c>
       <c r="AC6" t="str">
-        <f t="shared" ref="AC6:AC69" si="13">TEXT(U6, "0.00") &amp; "  (" &amp; TEXT( U7, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC6" si="13">TEXT(U6, "0.00") &amp; "  (" &amp; TEXT( U7, "0.00") &amp; ")"</f>
         <v>85.80  (1.43)</v>
       </c>
       <c r="AD6" t="str">
-        <f t="shared" ref="AD6:AD69" si="14">TEXT(V6, "0.00") &amp; "  (" &amp; TEXT( V7, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD6" si="14">TEXT(V6, "0.00") &amp; "  (" &amp; TEXT( V7, "0.00") &amp; ")"</f>
         <v>82.23  (0.11)</v>
       </c>
       <c r="AE6" t="str">
-        <f t="shared" ref="AE6:AE69" si="15">TEXT(W6, "0.00") &amp; "  (" &amp; TEXT( W7, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE6" si="15">TEXT(W6, "0.00") &amp; "  (" &amp; TEXT( W7, "0.00") &amp; ")"</f>
         <v>0.92  (0.01)</v>
       </c>
     </row>
@@ -2068,31 +2078,31 @@
         <v>0.9214966867776202</v>
       </c>
       <c r="Y10" t="str">
-        <f t="shared" ref="Y10:Y41" si="29">TEXT(Q10, "0.00") &amp; "  (" &amp; TEXT( Q11, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y10" si="29">TEXT(Q10, "0.00") &amp; "  (" &amp; TEXT( Q11, "0.00") &amp; ")"</f>
         <v>0.47  (0.03)</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" ref="Z10:Z73" si="30">TEXT(R10, "0.00") &amp; "  (" &amp; TEXT( R11, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z10" si="30">TEXT(R10, "0.00") &amp; "  (" &amp; TEXT( R11, "0.00") &amp; ")"</f>
         <v>0.97  (0.00)</v>
       </c>
       <c r="AA10" t="str">
-        <f t="shared" ref="AA10:AA73" si="31">TEXT(S10, "0.00") &amp; "  (" &amp; TEXT( S11, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA10" si="31">TEXT(S10, "0.00") &amp; "  (" &amp; TEXT( S11, "0.00") &amp; ")"</f>
         <v>0.87  (0.02)</v>
       </c>
       <c r="AB10" t="str">
-        <f t="shared" ref="AB10:AB41" si="32">TEXT(T10, "0") &amp; "  (" &amp; TEXT( T11, "0") &amp; ")"</f>
+        <f t="shared" ref="AB10" si="32">TEXT(T10, "0") &amp; "  (" &amp; TEXT( T11, "0") &amp; ")"</f>
         <v>2239  (381)</v>
       </c>
       <c r="AC10" t="str">
-        <f t="shared" ref="AC10:AC73" si="33">TEXT(U10, "0.00") &amp; "  (" &amp; TEXT( U11, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC10" si="33">TEXT(U10, "0.00") &amp; "  (" &amp; TEXT( U11, "0.00") &amp; ")"</f>
         <v>86.59  (1.73)</v>
       </c>
       <c r="AD10" t="str">
-        <f t="shared" ref="AD10:AD73" si="34">TEXT(V10, "0.00") &amp; "  (" &amp; TEXT( V11, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD10" si="34">TEXT(V10, "0.00") &amp; "  (" &amp; TEXT( V11, "0.00") &amp; ")"</f>
         <v>83.01  (0.29)</v>
       </c>
       <c r="AE10" t="str">
-        <f t="shared" ref="AE10:AE73" si="35">TEXT(W10, "0.00") &amp; "  (" &amp; TEXT( W11, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE10" si="35">TEXT(W10, "0.00") &amp; "  (" &amp; TEXT( W11, "0.00") &amp; ")"</f>
         <v>0.92  (0.01)</v>
       </c>
     </row>
@@ -2334,31 +2344,31 @@
         <v>0.90581099363450301</v>
       </c>
       <c r="Y14" t="str">
-        <f t="shared" ref="Y14:Y45" si="49">TEXT(Q14, "0.00") &amp; "  (" &amp; TEXT( Q15, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y14" si="49">TEXT(Q14, "0.00") &amp; "  (" &amp; TEXT( Q15, "0.00") &amp; ")"</f>
         <v>0.41  (0.02)</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" ref="Z14:Z77" si="50">TEXT(R14, "0.00") &amp; "  (" &amp; TEXT( R15, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z14" si="50">TEXT(R14, "0.00") &amp; "  (" &amp; TEXT( R15, "0.00") &amp; ")"</f>
         <v>0.97  (0.00)</v>
       </c>
       <c r="AA14" t="str">
-        <f t="shared" ref="AA14:AA77" si="51">TEXT(S14, "0.00") &amp; "  (" &amp; TEXT( S15, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA14" si="51">TEXT(S14, "0.00") &amp; "  (" &amp; TEXT( S15, "0.00") &amp; ")"</f>
         <v>0.85  (0.02)</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" ref="AB14:AB45" si="52">TEXT(T14, "0") &amp; "  (" &amp; TEXT( T15, "0") &amp; ")"</f>
+        <f t="shared" ref="AB14" si="52">TEXT(T14, "0") &amp; "  (" &amp; TEXT( T15, "0") &amp; ")"</f>
         <v>4972  (834)</v>
       </c>
       <c r="AC14" t="str">
-        <f t="shared" ref="AC14:AC77" si="53">TEXT(U14, "0.00") &amp; "  (" &amp; TEXT( U15, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC14" si="53">TEXT(U14, "0.00") &amp; "  (" &amp; TEXT( U15, "0.00") &amp; ")"</f>
         <v>84.11  (1.30)</v>
       </c>
       <c r="AD14" t="str">
-        <f t="shared" ref="AD14:AD77" si="54">TEXT(V14, "0.00") &amp; "  (" &amp; TEXT( V15, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD14" si="54">TEXT(V14, "0.00") &amp; "  (" &amp; TEXT( V15, "0.00") &amp; ")"</f>
         <v>81.12  (0.13)</v>
       </c>
       <c r="AE14" t="str">
-        <f t="shared" ref="AE14:AE77" si="55">TEXT(W14, "0.00") &amp; "  (" &amp; TEXT( W15, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE14" si="55">TEXT(W14, "0.00") &amp; "  (" &amp; TEXT( W15, "0.00") &amp; ")"</f>
         <v>0.91  (0.01)</v>
       </c>
     </row>
@@ -2600,31 +2610,31 @@
         <v>0.89387973062237158</v>
       </c>
       <c r="Y18" t="str">
-        <f t="shared" ref="Y18:Y49" si="69">TEXT(Q18, "0.00") &amp; "  (" &amp; TEXT( Q19, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y18" si="69">TEXT(Q18, "0.00") &amp; "  (" &amp; TEXT( Q19, "0.00") &amp; ")"</f>
         <v>0.15  (0.02)</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" ref="Z18:Z81" si="70">TEXT(R18, "0.00") &amp; "  (" &amp; TEXT( R19, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z18" si="70">TEXT(R18, "0.00") &amp; "  (" &amp; TEXT( R19, "0.00") &amp; ")"</f>
         <v>0.99  (0.00)</v>
       </c>
       <c r="AA18" t="str">
-        <f t="shared" ref="AA18:AA81" si="71">TEXT(S18, "0.00") &amp; "  (" &amp; TEXT( S19, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA18" si="71">TEXT(S18, "0.00") &amp; "  (" &amp; TEXT( S19, "0.00") &amp; ")"</f>
         <v>0.82  (0.04)</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" ref="AB18:AB49" si="72">TEXT(T18, "0") &amp; "  (" &amp; TEXT( T19, "0") &amp; ")"</f>
+        <f t="shared" ref="AB18" si="72">TEXT(T18, "0") &amp; "  (" &amp; TEXT( T19, "0") &amp; ")"</f>
         <v>2657  (342)</v>
       </c>
       <c r="AC18" t="str">
-        <f t="shared" ref="AC18:AC81" si="73">TEXT(U18, "0.00") &amp; "  (" &amp; TEXT( U19, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC18" si="73">TEXT(U18, "0.00") &amp; "  (" &amp; TEXT( U19, "0.00") &amp; ")"</f>
         <v>81.34  (3.58)</v>
       </c>
       <c r="AD18" t="str">
-        <f t="shared" ref="AD18:AD81" si="74">TEXT(V18, "0.00") &amp; "  (" &amp; TEXT( V19, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD18" si="74">TEXT(V18, "0.00") &amp; "  (" &amp; TEXT( V19, "0.00") &amp; ")"</f>
         <v>75.07  (0.59)</v>
       </c>
       <c r="AE18" t="str">
-        <f t="shared" ref="AE18:AE81" si="75">TEXT(W18, "0.00") &amp; "  (" &amp; TEXT( W19, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE18" si="75">TEXT(W18, "0.00") &amp; "  (" &amp; TEXT( W19, "0.00") &amp; ")"</f>
         <v>0.89  (0.02)</v>
       </c>
     </row>
@@ -2866,31 +2876,31 @@
         <v>0.88792727100504454</v>
       </c>
       <c r="Y22" t="str">
-        <f t="shared" ref="Y22:Y53" si="89">TEXT(Q22, "0.00") &amp; "  (" &amp; TEXT( Q23, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y22" si="89">TEXT(Q22, "0.00") &amp; "  (" &amp; TEXT( Q23, "0.00") &amp; ")"</f>
         <v>0.15  (0.02)</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" ref="Z22:Z81" si="90">TEXT(R22, "0.00") &amp; "  (" &amp; TEXT( R23, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z22" si="90">TEXT(R22, "0.00") &amp; "  (" &amp; TEXT( R23, "0.00") &amp; ")"</f>
         <v>0.99  (0.00)</v>
       </c>
       <c r="AA22" t="str">
-        <f t="shared" ref="AA22:AA81" si="91">TEXT(S22, "0.00") &amp; "  (" &amp; TEXT( S23, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA22" si="91">TEXT(S22, "0.00") &amp; "  (" &amp; TEXT( S23, "0.00") &amp; ")"</f>
         <v>0.81  (0.03)</v>
       </c>
       <c r="AB22" t="str">
-        <f t="shared" ref="AB22:AB53" si="92">TEXT(T22, "0") &amp; "  (" &amp; TEXT( T23, "0") &amp; ")"</f>
+        <f t="shared" ref="AB22" si="92">TEXT(T22, "0") &amp; "  (" &amp; TEXT( T23, "0") &amp; ")"</f>
         <v>2670  (366)</v>
       </c>
       <c r="AC22" t="str">
-        <f t="shared" ref="AC22:AC81" si="93">TEXT(U22, "0.00") &amp; "  (" &amp; TEXT( U23, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC22" si="93">TEXT(U22, "0.00") &amp; "  (" &amp; TEXT( U23, "0.00") &amp; ")"</f>
         <v>80.38  (3.18)</v>
       </c>
       <c r="AD22" t="str">
-        <f t="shared" ref="AD22:AD81" si="94">TEXT(V22, "0.00") &amp; "  (" &amp; TEXT( V23, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD22" si="94">TEXT(V22, "0.00") &amp; "  (" &amp; TEXT( V23, "0.00") &amp; ")"</f>
         <v>74.69  (0.99)</v>
       </c>
       <c r="AE22" t="str">
-        <f t="shared" ref="AE22:AE81" si="95">TEXT(W22, "0.00") &amp; "  (" &amp; TEXT( W23, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE22" si="95">TEXT(W22, "0.00") &amp; "  (" &amp; TEXT( W23, "0.00") &amp; ")"</f>
         <v>0.89  (0.02)</v>
       </c>
     </row>
@@ -3132,31 +3142,31 @@
         <v>0.8865798673597387</v>
       </c>
       <c r="Y26" t="str">
-        <f t="shared" ref="Y26:Y57" si="109">TEXT(Q26, "0.00") &amp; "  (" &amp; TEXT( Q27, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y26" si="109">TEXT(Q26, "0.00") &amp; "  (" &amp; TEXT( Q27, "0.00") &amp; ")"</f>
         <v>0.14  (0.01)</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" ref="Z26:Z81" si="110">TEXT(R26, "0.00") &amp; "  (" &amp; TEXT( R27, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z26" si="110">TEXT(R26, "0.00") &amp; "  (" &amp; TEXT( R27, "0.00") &amp; ")"</f>
         <v>0.99  (0.00)</v>
       </c>
       <c r="AA26" t="str">
-        <f t="shared" ref="AA26:AA81" si="111">TEXT(S26, "0.00") &amp; "  (" &amp; TEXT( S27, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA26" si="111">TEXT(S26, "0.00") &amp; "  (" &amp; TEXT( S27, "0.00") &amp; ")"</f>
         <v>0.81  (0.02)</v>
       </c>
       <c r="AB26" t="str">
-        <f t="shared" ref="AB26:AB57" si="112">TEXT(T26, "0") &amp; "  (" &amp; TEXT( T27, "0") &amp; ")"</f>
+        <f t="shared" ref="AB26" si="112">TEXT(T26, "0") &amp; "  (" &amp; TEXT( T27, "0") &amp; ")"</f>
         <v>2605  (396)</v>
       </c>
       <c r="AC26" t="str">
-        <f t="shared" ref="AC26:AC81" si="113">TEXT(U26, "0.00") &amp; "  (" &amp; TEXT( U27, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC26" si="113">TEXT(U26, "0.00") &amp; "  (" &amp; TEXT( U27, "0.00") &amp; ")"</f>
         <v>80.12  (1.62)</v>
       </c>
       <c r="AD26" t="str">
-        <f t="shared" ref="AD26:AD81" si="114">TEXT(V26, "0.00") &amp; "  (" &amp; TEXT( V27, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD26" si="114">TEXT(V26, "0.00") &amp; "  (" &amp; TEXT( V27, "0.00") &amp; ")"</f>
         <v>74.13  (0.42)</v>
       </c>
       <c r="AE26" t="str">
-        <f t="shared" ref="AE26:AE81" si="115">TEXT(W26, "0.00") &amp; "  (" &amp; TEXT( W27, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE26" si="115">TEXT(W26, "0.00") &amp; "  (" &amp; TEXT( W27, "0.00") &amp; ")"</f>
         <v>0.89  (0.01)</v>
       </c>
     </row>
@@ -3398,31 +3408,31 @@
         <v>0.89373502227219359</v>
       </c>
       <c r="Y30" t="str">
-        <f t="shared" ref="Y30:Y61" si="129">TEXT(Q30, "0.00") &amp; "  (" &amp; TEXT( Q31, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y30" si="129">TEXT(Q30, "0.00") &amp; "  (" &amp; TEXT( Q31, "0.00") &amp; ")"</f>
         <v>0.15  (0.01)</v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" ref="Z30:Z81" si="130">TEXT(R30, "0.00") &amp; "  (" &amp; TEXT( R31, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z30" si="130">TEXT(R30, "0.00") &amp; "  (" &amp; TEXT( R31, "0.00") &amp; ")"</f>
         <v>0.99  (0.00)</v>
       </c>
       <c r="AA30" t="str">
-        <f t="shared" ref="AA30:AA81" si="131">TEXT(S30, "0.00") &amp; "  (" &amp; TEXT( S31, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA30" si="131">TEXT(S30, "0.00") &amp; "  (" &amp; TEXT( S31, "0.00") &amp; ")"</f>
         <v>0.82  (0.01)</v>
       </c>
       <c r="AB30" t="str">
-        <f t="shared" ref="AB30:AB61" si="132">TEXT(T30, "0") &amp; "  (" &amp; TEXT( T31, "0") &amp; ")"</f>
+        <f t="shared" ref="AB30" si="132">TEXT(T30, "0") &amp; "  (" &amp; TEXT( T31, "0") &amp; ")"</f>
         <v>4932  (235)</v>
       </c>
       <c r="AC30" t="str">
-        <f t="shared" ref="AC30:AC81" si="133">TEXT(U30, "0.00") &amp; "  (" &amp; TEXT( U31, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC30" si="133">TEXT(U30, "0.00") &amp; "  (" &amp; TEXT( U31, "0.00") &amp; ")"</f>
         <v>81.24  (0.98)</v>
       </c>
       <c r="AD30" t="str">
-        <f t="shared" ref="AD30:AD81" si="134">TEXT(V30, "0.00") &amp; "  (" &amp; TEXT( V31, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD30" si="134">TEXT(V30, "0.00") &amp; "  (" &amp; TEXT( V31, "0.00") &amp; ")"</f>
         <v>74.55  (0.18)</v>
       </c>
       <c r="AE30" t="str">
-        <f t="shared" ref="AE30:AE81" si="135">TEXT(W30, "0.00") &amp; "  (" &amp; TEXT( W31, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE30" si="135">TEXT(W30, "0.00") &amp; "  (" &amp; TEXT( W31, "0.00") &amp; ")"</f>
         <v>0.89  (0.01)</v>
       </c>
     </row>
@@ -3664,31 +3674,31 @@
         <v>0.25079082812006603</v>
       </c>
       <c r="Y34" t="str">
-        <f t="shared" ref="Y34:Y81" si="149">TEXT(Q34, "0.00") &amp; "  (" &amp; TEXT( Q35, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y34" si="149">TEXT(Q34, "0.00") &amp; "  (" &amp; TEXT( Q35, "0.00") &amp; ")"</f>
         <v>0.17  (0.03)</v>
       </c>
       <c r="Z34" t="str">
-        <f t="shared" ref="Z34:Z81" si="150">TEXT(R34, "0.00") &amp; "  (" &amp; TEXT( R35, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z34" si="150">TEXT(R34, "0.00") &amp; "  (" &amp; TEXT( R35, "0.00") &amp; ")"</f>
         <v>0.16  (0.02)</v>
       </c>
       <c r="AA34" t="str">
-        <f t="shared" ref="AA34:AA81" si="151">TEXT(S34, "0.00") &amp; "  (" &amp; TEXT( S35, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA34" si="151">TEXT(S34, "0.00") &amp; "  (" &amp; TEXT( S35, "0.00") &amp; ")"</f>
         <v>0.67  (0.07)</v>
       </c>
       <c r="AB34" t="str">
-        <f t="shared" ref="AB34:AB81" si="152">TEXT(T34, "0") &amp; "  (" &amp; TEXT( T35, "0") &amp; ")"</f>
+        <f t="shared" ref="AB34" si="152">TEXT(T34, "0") &amp; "  (" &amp; TEXT( T35, "0") &amp; ")"</f>
         <v>2857  (583)</v>
       </c>
       <c r="AC34" t="str">
-        <f t="shared" ref="AC34:AC81" si="153">TEXT(U34, "0.00") &amp; "  (" &amp; TEXT( U35, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC34" si="153">TEXT(U34, "0.00") &amp; "  (" &amp; TEXT( U35, "0.00") &amp; ")"</f>
         <v>76.50  (5.63)</v>
       </c>
       <c r="AD34" t="str">
-        <f t="shared" ref="AD34:AD81" si="154">TEXT(V34, "0.00") &amp; "  (" &amp; TEXT( V35, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD34" si="154">TEXT(V34, "0.00") &amp; "  (" &amp; TEXT( V35, "0.00") &amp; ")"</f>
         <v>72.16  (0.51)</v>
       </c>
       <c r="AE34" t="str">
-        <f t="shared" ref="AE34:AE81" si="155">TEXT(W34, "0.00") &amp; "  (" &amp; TEXT( W35, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE34" si="155">TEXT(W34, "0.00") &amp; "  (" &amp; TEXT( W35, "0.00") &amp; ")"</f>
         <v>0.25  (0.03)</v>
       </c>
     </row>
@@ -3906,7 +3916,7 @@
         <v>0.20660717741963275</v>
       </c>
       <c r="R38">
-        <f t="shared" ref="Q38:R38" si="163">AVERAGE(I38:I41)</f>
+        <f t="shared" ref="R38" si="163">AVERAGE(I38:I41)</f>
         <v>0.17836492351064526</v>
       </c>
       <c r="S38">
@@ -3930,31 +3940,31 @@
         <v>0.277134389048728</v>
       </c>
       <c r="Y38" t="str">
-        <f t="shared" ref="Y38:Y81" si="169">TEXT(Q38, "0.00") &amp; "  (" &amp; TEXT( Q39, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y38" si="169">TEXT(Q38, "0.00") &amp; "  (" &amp; TEXT( Q39, "0.00") &amp; ")"</f>
         <v>0.21  (0.03)</v>
       </c>
       <c r="Z38" t="str">
-        <f t="shared" ref="Z38:Z81" si="170">TEXT(R38, "0.00") &amp; "  (" &amp; TEXT( R39, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z38" si="170">TEXT(R38, "0.00") &amp; "  (" &amp; TEXT( R39, "0.00") &amp; ")"</f>
         <v>0.18  (0.02)</v>
       </c>
       <c r="AA38" t="str">
-        <f t="shared" ref="AA38:AA81" si="171">TEXT(S38, "0.00") &amp; "  (" &amp; TEXT( S39, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA38" si="171">TEXT(S38, "0.00") &amp; "  (" &amp; TEXT( S39, "0.00") &amp; ")"</f>
         <v>0.64  (0.05)</v>
       </c>
       <c r="AB38" t="str">
-        <f t="shared" ref="AB38:AB81" si="172">TEXT(T38, "0") &amp; "  (" &amp; TEXT( T39, "0") &amp; ")"</f>
+        <f t="shared" ref="AB38" si="172">TEXT(T38, "0") &amp; "  (" &amp; TEXT( T39, "0") &amp; ")"</f>
         <v>2877  (690)</v>
       </c>
       <c r="AC38" t="str">
-        <f t="shared" ref="AC38:AC81" si="173">TEXT(U38, "0.00") &amp; "  (" &amp; TEXT( U39, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC38" si="173">TEXT(U38, "0.00") &amp; "  (" &amp; TEXT( U39, "0.00") &amp; ")"</f>
         <v>80.77  (3.30)</v>
       </c>
       <c r="AD38" t="str">
-        <f t="shared" ref="AD38:AD81" si="174">TEXT(V38, "0.00") &amp; "  (" &amp; TEXT( V39, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD38" si="174">TEXT(V38, "0.00") &amp; "  (" &amp; TEXT( V39, "0.00") &amp; ")"</f>
         <v>72.83  (0.53)</v>
       </c>
       <c r="AE38" t="str">
-        <f t="shared" ref="AE38:AE81" si="175">TEXT(W38, "0.00") &amp; "  (" &amp; TEXT( W39, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE38" si="175">TEXT(W38, "0.00") &amp; "  (" &amp; TEXT( W39, "0.00") &amp; ")"</f>
         <v>0.28  (0.02)</v>
       </c>
     </row>
@@ -4196,31 +4206,31 @@
         <v>0.24933753416052001</v>
       </c>
       <c r="Y42" t="str">
-        <f t="shared" ref="Y42:Y81" si="189">TEXT(Q42, "0.00") &amp; "  (" &amp; TEXT( Q43, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y42" si="189">TEXT(Q42, "0.00") &amp; "  (" &amp; TEXT( Q43, "0.00") &amp; ")"</f>
         <v>0.17  (0.01)</v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" ref="Z42:Z81" si="190">TEXT(R42, "0.00") &amp; "  (" &amp; TEXT( R43, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z42" si="190">TEXT(R42, "0.00") &amp; "  (" &amp; TEXT( R43, "0.00") &amp; ")"</f>
         <v>0.15  (0.01)</v>
       </c>
       <c r="AA42" t="str">
-        <f t="shared" ref="AA42:AA81" si="191">TEXT(S42, "0.00") &amp; "  (" &amp; TEXT( S43, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA42" si="191">TEXT(S42, "0.00") &amp; "  (" &amp; TEXT( S43, "0.00") &amp; ")"</f>
         <v>0.68  (0.02)</v>
       </c>
       <c r="AB42" t="str">
-        <f t="shared" ref="AB42:AB81" si="192">TEXT(T42, "0") &amp; "  (" &amp; TEXT( T43, "0") &amp; ")"</f>
+        <f t="shared" ref="AB42" si="192">TEXT(T42, "0") &amp; "  (" &amp; TEXT( T43, "0") &amp; ")"</f>
         <v>2732  (444)</v>
       </c>
       <c r="AC42" t="str">
-        <f t="shared" ref="AC42:AC81" si="193">TEXT(U42, "0.00") &amp; "  (" &amp; TEXT( U43, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC42" si="193">TEXT(U42, "0.00") &amp; "  (" &amp; TEXT( U43, "0.00") &amp; ")"</f>
         <v>76.75  (1.51)</v>
       </c>
       <c r="AD42" t="str">
-        <f t="shared" ref="AD42:AD81" si="194">TEXT(V42, "0.00") &amp; "  (" &amp; TEXT( V43, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD42" si="194">TEXT(V42, "0.00") &amp; "  (" &amp; TEXT( V43, "0.00") &amp; ")"</f>
         <v>72.54  (0.47)</v>
       </c>
       <c r="AE42" t="str">
-        <f t="shared" ref="AE42:AE81" si="195">TEXT(W42, "0.00") &amp; "  (" &amp; TEXT( W43, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE42" si="195">TEXT(W42, "0.00") &amp; "  (" &amp; TEXT( W43, "0.00") &amp; ")"</f>
         <v>0.25  (0.01)</v>
       </c>
     </row>
@@ -4462,31 +4472,31 @@
         <v>0.25099673022200175</v>
       </c>
       <c r="Y46" t="str">
-        <f t="shared" ref="Y46:Y81" si="209">TEXT(Q46, "0.00") &amp; "  (" &amp; TEXT( Q47, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y46" si="209">TEXT(Q46, "0.00") &amp; "  (" &amp; TEXT( Q47, "0.00") &amp; ")"</f>
         <v>0.17  (0.03)</v>
       </c>
       <c r="Z46" t="str">
-        <f t="shared" ref="Z46:Z81" si="210">TEXT(R46, "0.00") &amp; "  (" &amp; TEXT( R47, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z46" si="210">TEXT(R46, "0.00") &amp; "  (" &amp; TEXT( R47, "0.00") &amp; ")"</f>
         <v>0.16  (0.02)</v>
       </c>
       <c r="AA46" t="str">
-        <f t="shared" ref="AA46:AA81" si="211">TEXT(S46, "0.00") &amp; "  (" &amp; TEXT( S47, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA46" si="211">TEXT(S46, "0.00") &amp; "  (" &amp; TEXT( S47, "0.00") &amp; ")"</f>
         <v>0.68  (0.06)</v>
       </c>
       <c r="AB46" t="str">
-        <f t="shared" ref="AB46:AB81" si="212">TEXT(T46, "0") &amp; "  (" &amp; TEXT( T47, "0") &amp; ")"</f>
+        <f t="shared" ref="AB46" si="212">TEXT(T46, "0") &amp; "  (" &amp; TEXT( T47, "0") &amp; ")"</f>
         <v>5092  (343)</v>
       </c>
       <c r="AC46" t="str">
-        <f t="shared" ref="AC46:AC81" si="213">TEXT(U46, "0.00") &amp; "  (" &amp; TEXT( U47, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC46" si="213">TEXT(U46, "0.00") &amp; "  (" &amp; TEXT( U47, "0.00") &amp; ")"</f>
         <v>76.38  (5.65)</v>
       </c>
       <c r="AD46" t="str">
-        <f t="shared" ref="AD46:AD81" si="214">TEXT(V46, "0.00") &amp; "  (" &amp; TEXT( V47, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD46" si="214">TEXT(V46, "0.00") &amp; "  (" &amp; TEXT( V47, "0.00") &amp; ")"</f>
         <v>72.35  (0.42)</v>
       </c>
       <c r="AE46" t="str">
-        <f t="shared" ref="AE46:AE81" si="215">TEXT(W46, "0.00") &amp; "  (" &amp; TEXT( W47, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE46" si="215">TEXT(W46, "0.00") &amp; "  (" &amp; TEXT( W47, "0.00") &amp; ")"</f>
         <v>0.25  (0.02)</v>
       </c>
     </row>
@@ -4728,31 +4738,31 @@
         <v>0.78880707991989718</v>
       </c>
       <c r="Y50" t="str">
-        <f t="shared" ref="Y50:Y81" si="229">TEXT(Q50, "0.00") &amp; "  (" &amp; TEXT( Q51, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y50" si="229">TEXT(Q50, "0.00") &amp; "  (" &amp; TEXT( Q51, "0.00") &amp; ")"</f>
         <v>0.08  (0.01)</v>
       </c>
       <c r="Z50" t="str">
-        <f t="shared" ref="Z50:Z81" si="230">TEXT(R50, "0.00") &amp; "  (" &amp; TEXT( R51, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z50" si="230">TEXT(R50, "0.00") &amp; "  (" &amp; TEXT( R51, "0.00") &amp; ")"</f>
         <v>0.98  (0.00)</v>
       </c>
       <c r="AA50" t="str">
-        <f t="shared" ref="AA50:AA81" si="231">TEXT(S50, "0.00") &amp; "  (" &amp; TEXT( S51, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA50" si="231">TEXT(S50, "0.00") &amp; "  (" &amp; TEXT( S51, "0.00") &amp; ")"</f>
         <v>0.66  (0.05)</v>
       </c>
       <c r="AB50" t="str">
-        <f t="shared" ref="AB50:AB81" si="232">TEXT(T50, "0") &amp; "  (" &amp; TEXT( T51, "0") &amp; ")"</f>
+        <f t="shared" ref="AB50" si="232">TEXT(T50, "0") &amp; "  (" &amp; TEXT( T51, "0") &amp; ")"</f>
         <v>1907  (724)</v>
       </c>
       <c r="AC50" t="str">
-        <f t="shared" ref="AC50:AC81" si="233">TEXT(U50, "0.00") &amp; "  (" &amp; TEXT( U51, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC50" si="233">TEXT(U50, "0.00") &amp; "  (" &amp; TEXT( U51, "0.00") &amp; ")"</f>
         <v>66.26  (4.62)</v>
       </c>
       <c r="AD50" t="str">
-        <f t="shared" ref="AD50:AD81" si="234">TEXT(V50, "0.00") &amp; "  (" &amp; TEXT( V51, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD50" si="234">TEXT(V50, "0.00") &amp; "  (" &amp; TEXT( V51, "0.00") &amp; ")"</f>
         <v>69.23  (0.19)</v>
       </c>
       <c r="AE50" t="str">
-        <f t="shared" ref="AE50:AE81" si="235">TEXT(W50, "0.00") &amp; "  (" &amp; TEXT( W51, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE50" si="235">TEXT(W50, "0.00") &amp; "  (" &amp; TEXT( W51, "0.00") &amp; ")"</f>
         <v>0.79  (0.04)</v>
       </c>
     </row>
@@ -4994,31 +5004,31 @@
         <v>0.80935153986784247</v>
       </c>
       <c r="Y54" t="str">
-        <f t="shared" ref="Y54:Y81" si="249">TEXT(Q54, "0.00") &amp; "  (" &amp; TEXT( Q55, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y54" si="249">TEXT(Q54, "0.00") &amp; "  (" &amp; TEXT( Q55, "0.00") &amp; ")"</f>
         <v>0.09  (0.01)</v>
       </c>
       <c r="Z54" t="str">
-        <f t="shared" ref="Z54:Z81" si="250">TEXT(R54, "0.00") &amp; "  (" &amp; TEXT( R55, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z54" si="250">TEXT(R54, "0.00") &amp; "  (" &amp; TEXT( R55, "0.00") &amp; ")"</f>
         <v>0.98  (0.00)</v>
       </c>
       <c r="AA54" t="str">
-        <f t="shared" ref="AA54:AA81" si="251">TEXT(S54, "0.00") &amp; "  (" &amp; TEXT( S55, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA54" si="251">TEXT(S54, "0.00") &amp; "  (" &amp; TEXT( S55, "0.00") &amp; ")"</f>
         <v>0.69  (0.06)</v>
       </c>
       <c r="AB54" t="str">
-        <f t="shared" ref="AB54:AB81" si="252">TEXT(T54, "0") &amp; "  (" &amp; TEXT( T55, "0") &amp; ")"</f>
+        <f t="shared" ref="AB54" si="252">TEXT(T54, "0") &amp; "  (" &amp; TEXT( T55, "0") &amp; ")"</f>
         <v>2122  (323)</v>
       </c>
       <c r="AC54" t="str">
-        <f t="shared" ref="AC54:AC81" si="253">TEXT(U54, "0.00") &amp; "  (" &amp; TEXT( U55, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC54" si="253">TEXT(U54, "0.00") &amp; "  (" &amp; TEXT( U55, "0.00") &amp; ")"</f>
         <v>69.06  (5.13)</v>
       </c>
       <c r="AD54" t="str">
-        <f t="shared" ref="AD54:AD81" si="254">TEXT(V54, "0.00") &amp; "  (" &amp; TEXT( V55, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD54" si="254">TEXT(V54, "0.00") &amp; "  (" &amp; TEXT( V55, "0.00") &amp; ")"</f>
         <v>70.72  (0.41)</v>
       </c>
       <c r="AE54" t="str">
-        <f t="shared" ref="AE54:AE81" si="255">TEXT(W54, "0.00") &amp; "  (" &amp; TEXT( W55, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE54" si="255">TEXT(W54, "0.00") &amp; "  (" &amp; TEXT( W55, "0.00") &amp; ")"</f>
         <v>0.81  (0.04)</v>
       </c>
     </row>
@@ -5260,31 +5270,31 @@
         <v>0.86857938291109227</v>
       </c>
       <c r="Y58" t="str">
-        <f t="shared" ref="Y58:Y81" si="269">TEXT(Q58, "0.00") &amp; "  (" &amp; TEXT( Q59, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y58" si="269">TEXT(Q58, "0.00") &amp; "  (" &amp; TEXT( Q59, "0.00") &amp; ")"</f>
         <v>0.11  (0.00)</v>
       </c>
       <c r="Z58" t="str">
-        <f t="shared" ref="Z58:Z81" si="270">TEXT(R58, "0.00") &amp; "  (" &amp; TEXT( R59, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z58" si="270">TEXT(R58, "0.00") &amp; "  (" &amp; TEXT( R59, "0.00") &amp; ")"</f>
         <v>0.98  (0.00)</v>
       </c>
       <c r="AA58" t="str">
-        <f t="shared" ref="AA58:AA81" si="271">TEXT(S58, "0.00") &amp; "  (" &amp; TEXT( S59, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA58" si="271">TEXT(S58, "0.00") &amp; "  (" &amp; TEXT( S59, "0.00") &amp; ")"</f>
         <v>0.78  (0.03)</v>
       </c>
       <c r="AB58" t="str">
-        <f t="shared" ref="AB58:AB81" si="272">TEXT(T58, "0") &amp; "  (" &amp; TEXT( T59, "0") &amp; ")"</f>
+        <f t="shared" ref="AB58" si="272">TEXT(T58, "0") &amp; "  (" &amp; TEXT( T59, "0") &amp; ")"</f>
         <v>2158  (355)</v>
       </c>
       <c r="AC58" t="str">
-        <f t="shared" ref="AC58:AC81" si="273">TEXT(U58, "0.00") &amp; "  (" &amp; TEXT( U59, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC58" si="273">TEXT(U58, "0.00") &amp; "  (" &amp; TEXT( U59, "0.00") &amp; ")"</f>
         <v>77.33  (2.31)</v>
       </c>
       <c r="AD58" t="str">
-        <f t="shared" ref="AD58:AD81" si="274">TEXT(V58, "0.00") &amp; "  (" &amp; TEXT( V59, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD58" si="274">TEXT(V58, "0.00") &amp; "  (" &amp; TEXT( V59, "0.00") &amp; ")"</f>
         <v>68.03  (1.21)</v>
       </c>
       <c r="AE58" t="str">
-        <f t="shared" ref="AE58:AE81" si="275">TEXT(W58, "0.00") &amp; "  (" &amp; TEXT( W59, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE58" si="275">TEXT(W58, "0.00") &amp; "  (" &amp; TEXT( W59, "0.00") &amp; ")"</f>
         <v>0.87  (0.02)</v>
       </c>
     </row>
@@ -5526,31 +5536,31 @@
         <v>0.85225877961291974</v>
       </c>
       <c r="Y62" t="str">
-        <f t="shared" ref="Y62:Y81" si="289">TEXT(Q62, "0.00") &amp; "  (" &amp; TEXT( Q63, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y62" si="289">TEXT(Q62, "0.00") &amp; "  (" &amp; TEXT( Q63, "0.00") &amp; ")"</f>
         <v>0.11  (0.01)</v>
       </c>
       <c r="Z62" t="str">
-        <f t="shared" ref="Z62:Z81" si="290">TEXT(R62, "0.00") &amp; "  (" &amp; TEXT( R63, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z62" si="290">TEXT(R62, "0.00") &amp; "  (" &amp; TEXT( R63, "0.00") &amp; ")"</f>
         <v>0.98  (0.00)</v>
       </c>
       <c r="AA62" t="str">
-        <f t="shared" ref="AA62:AA81" si="291">TEXT(S62, "0.00") &amp; "  (" &amp; TEXT( S63, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA62" si="291">TEXT(S62, "0.00") &amp; "  (" &amp; TEXT( S63, "0.00") &amp; ")"</f>
         <v>0.76  (0.05)</v>
       </c>
       <c r="AB62" t="str">
-        <f t="shared" ref="AB62:AB81" si="292">TEXT(T62, "0") &amp; "  (" &amp; TEXT( T63, "0") &amp; ")"</f>
+        <f t="shared" ref="AB62" si="292">TEXT(T62, "0") &amp; "  (" &amp; TEXT( T63, "0") &amp; ")"</f>
         <v>4370  (675)</v>
       </c>
       <c r="AC62" t="str">
-        <f t="shared" ref="AC62:AC81" si="293">TEXT(U62, "0.00") &amp; "  (" &amp; TEXT( U63, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC62" si="293">TEXT(U62, "0.00") &amp; "  (" &amp; TEXT( U63, "0.00") &amp; ")"</f>
         <v>75.03  (4.73)</v>
       </c>
       <c r="AD62" t="str">
-        <f t="shared" ref="AD62:AD81" si="294">TEXT(V62, "0.00") &amp; "  (" &amp; TEXT( V63, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD62" si="294">TEXT(V62, "0.00") &amp; "  (" &amp; TEXT( V63, "0.00") &amp; ")"</f>
         <v>69.18  (1.04)</v>
       </c>
       <c r="AE62" t="str">
-        <f t="shared" ref="AE62:AE81" si="295">TEXT(W62, "0.00") &amp; "  (" &amp; TEXT( W63, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE62" si="295">TEXT(W62, "0.00") &amp; "  (" &amp; TEXT( W63, "0.00") &amp; ")"</f>
         <v>0.85  (0.03)</v>
       </c>
     </row>
@@ -5792,31 +5802,31 @@
         <v>0.367124304922825</v>
       </c>
       <c r="Y66" t="str">
-        <f t="shared" ref="Y66:Y81" si="309">TEXT(Q66, "0.00") &amp; "  (" &amp; TEXT( Q67, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y66" si="309">TEXT(Q66, "0.00") &amp; "  (" &amp; TEXT( Q67, "0.00") &amp; ")"</f>
         <v>0.31  (0.03)</v>
       </c>
       <c r="Z66" t="str">
-        <f t="shared" ref="Z66:Z81" si="310">TEXT(R66, "0.00") &amp; "  (" &amp; TEXT( R67, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z66" si="310">TEXT(R66, "0.00") &amp; "  (" &amp; TEXT( R67, "0.00") &amp; ")"</f>
         <v>0.24  (0.02)</v>
       </c>
       <c r="AA66" t="str">
-        <f t="shared" ref="AA66:AA81" si="311">TEXT(S66, "0.00") &amp; "  (" &amp; TEXT( S67, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA66" si="311">TEXT(S66, "0.00") &amp; "  (" &amp; TEXT( S67, "0.00") &amp; ")"</f>
         <v>0.77  (0.02)</v>
       </c>
       <c r="AB66" t="str">
-        <f t="shared" ref="AB66:AB81" si="312">TEXT(T66, "0") &amp; "  (" &amp; TEXT( T67, "0") &amp; ")"</f>
+        <f t="shared" ref="AB66" si="312">TEXT(T66, "0") &amp; "  (" &amp; TEXT( T67, "0") &amp; ")"</f>
         <v>2430  (232)</v>
       </c>
       <c r="AC66" t="str">
-        <f t="shared" ref="AC66:AC81" si="313">TEXT(U66, "0.00") &amp; "  (" &amp; TEXT( U67, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC66" si="313">TEXT(U66, "0.00") &amp; "  (" &amp; TEXT( U67, "0.00") &amp; ")"</f>
         <v>85.68  (1.76)</v>
       </c>
       <c r="AD66" t="str">
-        <f t="shared" ref="AD66:AD81" si="314">TEXT(V66, "0.00") &amp; "  (" &amp; TEXT( V67, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD66" si="314">TEXT(V66, "0.00") &amp; "  (" &amp; TEXT( V67, "0.00") &amp; ")"</f>
         <v>81.48  (0.32)</v>
       </c>
       <c r="AE66" t="str">
-        <f t="shared" ref="AE66:AE81" si="315">TEXT(W66, "0.00") &amp; "  (" &amp; TEXT( W67, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE66" si="315">TEXT(W66, "0.00") &amp; "  (" &amp; TEXT( W67, "0.00") &amp; ")"</f>
         <v>0.37  (0.02)</v>
       </c>
     </row>
@@ -6058,31 +6068,31 @@
         <v>0.38058513392288651</v>
       </c>
       <c r="Y70" t="str">
-        <f t="shared" ref="Y70:Y81" si="329">TEXT(Q70, "0.00") &amp; "  (" &amp; TEXT( Q71, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y70" si="329">TEXT(Q70, "0.00") &amp; "  (" &amp; TEXT( Q71, "0.00") &amp; ")"</f>
         <v>0.33  (0.04)</v>
       </c>
       <c r="Z70" t="str">
-        <f t="shared" ref="Z70:Z81" si="330">TEXT(R70, "0.00") &amp; "  (" &amp; TEXT( R71, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z70" si="330">TEXT(R70, "0.00") &amp; "  (" &amp; TEXT( R71, "0.00") &amp; ")"</f>
         <v>0.26  (0.03)</v>
       </c>
       <c r="AA70" t="str">
-        <f t="shared" ref="AA70:AA81" si="331">TEXT(S70, "0.00") &amp; "  (" &amp; TEXT( S71, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA70" si="331">TEXT(S70, "0.00") &amp; "  (" &amp; TEXT( S71, "0.00") &amp; ")"</f>
         <v>0.76  (0.03)</v>
       </c>
       <c r="AB70" t="str">
-        <f t="shared" ref="AB70:AB81" si="332">TEXT(T70, "0") &amp; "  (" &amp; TEXT( T71, "0") &amp; ")"</f>
+        <f t="shared" ref="AB70" si="332">TEXT(T70, "0") &amp; "  (" &amp; TEXT( T71, "0") &amp; ")"</f>
         <v>2334  (226)</v>
       </c>
       <c r="AC70" t="str">
-        <f t="shared" ref="AC70:AC81" si="333">TEXT(U70, "0.00") &amp; "  (" &amp; TEXT( U71, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC70" si="333">TEXT(U70, "0.00") &amp; "  (" &amp; TEXT( U71, "0.00") &amp; ")"</f>
         <v>86.54  (2.54)</v>
       </c>
       <c r="AD70" t="str">
-        <f t="shared" ref="AD70:AD81" si="334">TEXT(V70, "0.00") &amp; "  (" &amp; TEXT( V71, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD70" si="334">TEXT(V70, "0.00") &amp; "  (" &amp; TEXT( V71, "0.00") &amp; ")"</f>
         <v>81.39  (0.21)</v>
       </c>
       <c r="AE70" t="str">
-        <f t="shared" ref="AE70:AE81" si="335">TEXT(W70, "0.00") &amp; "  (" &amp; TEXT( W71, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE70" si="335">TEXT(W70, "0.00") &amp; "  (" &amp; TEXT( W71, "0.00") &amp; ")"</f>
         <v>0.38  (0.03)</v>
       </c>
     </row>
@@ -6324,31 +6334,31 @@
         <v>0.33552852470556049</v>
       </c>
       <c r="Y74" t="str">
-        <f t="shared" ref="Y74:Y81" si="349">TEXT(Q74, "0.00") &amp; "  (" &amp; TEXT( Q75, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y74" si="349">TEXT(Q74, "0.00") &amp; "  (" &amp; TEXT( Q75, "0.00") &amp; ")"</f>
         <v>0.27  (0.04)</v>
       </c>
       <c r="Z74" t="str">
-        <f t="shared" ref="Z74:Z81" si="350">TEXT(R74, "0.00") &amp; "  (" &amp; TEXT( R75, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z74" si="350">TEXT(R74, "0.00") &amp; "  (" &amp; TEXT( R75, "0.00") &amp; ")"</f>
         <v>0.22  (0.03)</v>
       </c>
       <c r="AA74" t="str">
-        <f t="shared" ref="AA74:AA81" si="351">TEXT(S74, "0.00") &amp; "  (" &amp; TEXT( S75, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA74" si="351">TEXT(S74, "0.00") &amp; "  (" &amp; TEXT( S75, "0.00") &amp; ")"</f>
         <v>0.78  (0.04)</v>
       </c>
       <c r="AB74" t="str">
-        <f t="shared" ref="AB74:AB81" si="352">TEXT(T74, "0") &amp; "  (" &amp; TEXT( T75, "0") &amp; ")"</f>
+        <f t="shared" ref="AB74" si="352">TEXT(T74, "0") &amp; "  (" &amp; TEXT( T75, "0") &amp; ")"</f>
         <v>2324  (234)</v>
       </c>
       <c r="AC74" t="str">
-        <f t="shared" ref="AC74:AC81" si="353">TEXT(U74, "0.00") &amp; "  (" &amp; TEXT( U75, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC74" si="353">TEXT(U74, "0.00") &amp; "  (" &amp; TEXT( U75, "0.00") &amp; ")"</f>
         <v>83.19  (3.01)</v>
       </c>
       <c r="AD74" t="str">
-        <f t="shared" ref="AD74:AD81" si="354">TEXT(V74, "0.00") &amp; "  (" &amp; TEXT( V75, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD74" si="354">TEXT(V74, "0.00") &amp; "  (" &amp; TEXT( V75, "0.00") &amp; ")"</f>
         <v>80.59  (0.29)</v>
       </c>
       <c r="AE74" t="str">
-        <f t="shared" ref="AE74:AE81" si="355">TEXT(W74, "0.00") &amp; "  (" &amp; TEXT( W75, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE74" si="355">TEXT(W74, "0.00") &amp; "  (" &amp; TEXT( W75, "0.00") &amp; ")"</f>
         <v>0.34  (0.03)</v>
       </c>
     </row>
@@ -6590,31 +6600,31 @@
         <v>0.35640404950820753</v>
       </c>
       <c r="Y78" t="str">
-        <f t="shared" ref="Y78:Y81" si="369">TEXT(Q78, "0.00") &amp; "  (" &amp; TEXT( Q79, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Y78" si="369">TEXT(Q78, "0.00") &amp; "  (" &amp; TEXT( Q79, "0.00") &amp; ")"</f>
         <v>0.30  (0.02)</v>
       </c>
       <c r="Z78" t="str">
-        <f t="shared" ref="Z78:Z81" si="370">TEXT(R78, "0.00") &amp; "  (" &amp; TEXT( R79, "0.00") &amp; ")"</f>
+        <f t="shared" ref="Z78" si="370">TEXT(R78, "0.00") &amp; "  (" &amp; TEXT( R79, "0.00") &amp; ")"</f>
         <v>0.23  (0.01)</v>
       </c>
       <c r="AA78" t="str">
-        <f t="shared" ref="AA78:AA81" si="371">TEXT(S78, "0.00") &amp; "  (" &amp; TEXT( S79, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AA78" si="371">TEXT(S78, "0.00") &amp; "  (" &amp; TEXT( S79, "0.00") &amp; ")"</f>
         <v>0.77  (0.01)</v>
       </c>
       <c r="AB78" t="str">
-        <f t="shared" ref="AB78:AB81" si="372">TEXT(T78, "0") &amp; "  (" &amp; TEXT( T79, "0") &amp; ")"</f>
+        <f t="shared" ref="AB78" si="372">TEXT(T78, "0") &amp; "  (" &amp; TEXT( T79, "0") &amp; ")"</f>
         <v>5180  (246)</v>
       </c>
       <c r="AC78" t="str">
-        <f t="shared" ref="AC78:AC81" si="373">TEXT(U78, "0.00") &amp; "  (" &amp; TEXT( U79, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AC78" si="373">TEXT(U78, "0.00") &amp; "  (" &amp; TEXT( U79, "0.00") &amp; ")"</f>
         <v>85.01  (1.07)</v>
       </c>
       <c r="AD78" t="str">
-        <f t="shared" ref="AD78:AD81" si="374">TEXT(V78, "0.00") &amp; "  (" &amp; TEXT( V79, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AD78" si="374">TEXT(V78, "0.00") &amp; "  (" &amp; TEXT( V79, "0.00") &amp; ")"</f>
         <v>81.31  (0.19)</v>
       </c>
       <c r="AE78" t="str">
-        <f t="shared" ref="AE78:AE81" si="375">TEXT(W78, "0.00") &amp; "  (" &amp; TEXT( W79, "0.00") &amp; ")"</f>
+        <f t="shared" ref="AE78" si="375">TEXT(W78, "0.00") &amp; "  (" &amp; TEXT( W79, "0.00") &amp; ")"</f>
         <v>0.36  (0.01)</v>
       </c>
     </row>
@@ -7419,10 +7429,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T37"/>
+  <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8061,60 +8071,60 @@
         <v>23</v>
       </c>
       <c r="R31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E32" t="s">
         <v>152</v>
       </c>
       <c r="F32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="H32" t="s">
         <v>152</v>
       </c>
       <c r="I32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="K32" t="s">
         <v>152</v>
       </c>
       <c r="L32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="N32" t="s">
         <v>152</v>
       </c>
       <c r="O32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="Q32" t="s">
         <v>152</v>
       </c>
       <c r="R32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S32" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="T32" t="s">
         <v>152</v>
@@ -8122,61 +8132,61 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="D33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
@@ -8382,12 +8392,183 @@
         <v>148</v>
       </c>
     </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" t="s">
+        <v>157</v>
+      </c>
+      <c r="H40" t="s">
+        <v>152</v>
+      </c>
+      <c r="I40" t="s">
+        <v>153</v>
+      </c>
+      <c r="J40" t="s">
+        <v>157</v>
+      </c>
+      <c r="K40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F43" t="s">
+        <v>136</v>
+      </c>
+      <c r="G43" t="s">
+        <v>135</v>
+      </c>
+      <c r="H43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" t="s">
+        <v>143</v>
+      </c>
+      <c r="G44" t="s">
+        <v>142</v>
+      </c>
+      <c r="H44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" t="s">
+        <v>120</v>
+      </c>
+      <c r="F45" t="s">
+        <v>150</v>
+      </c>
+      <c r="G45" t="s">
+        <v>149</v>
+      </c>
+      <c r="H45" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B18:B21">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:B37">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B34:B37">
+  <conditionalFormatting sqref="B42:B45">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>